<commit_message>
change profile pic,delete profile pic,pulsa telkomsel positive,pulsa telkomsel negative,paket data telkomsel positive,paket data telkomsel negative
</commit_message>
<xml_diff>
--- a/IOS/Bayar Beli - BPJS Kesehatan/Default.xlsx
+++ b/IOS/Bayar Beli - BPJS Kesehatan/Default.xlsx
@@ -249,10 +249,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="283845"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -623,7 +623,7 @@
     <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>